<commit_message>
V1 version finalizada a la espera de mas informacion en caso de que se deba corregir segun la consulta legal en la administracion de roles al ser el titular del contrato titular y viajero a la vez
</commit_message>
<xml_diff>
--- a/DatosViajeros.xlsx
+++ b/DatosViajeros.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DatosViajeros\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{477250C2-799C-4E27-84CA-EB1BDEDD5E64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{142C8FFA-FE43-4FB6-B375-E5FD2CF3E5E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5DF11FD6-0A61-4C2B-9CEC-54DEE1359997}"/>
   </bookViews>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="203">
   <si>
     <t>Nombre</t>
   </si>
@@ -621,174 +621,6 @@
   </si>
   <si>
     <t>Código del Municipio(Solo España)</t>
-  </si>
-  <si>
-    <t>Ana</t>
-  </si>
-  <si>
-    <t>López</t>
-  </si>
-  <si>
-    <t>García</t>
-  </si>
-  <si>
-    <t>DNI</t>
-  </si>
-  <si>
-    <t>11211211B</t>
-  </si>
-  <si>
-    <t>Carlos</t>
-  </si>
-  <si>
-    <t>Alvarez</t>
-  </si>
-  <si>
-    <t>Ramírez</t>
-  </si>
-  <si>
-    <t>11311311C</t>
-  </si>
-  <si>
-    <t>Laura</t>
-  </si>
-  <si>
-    <t>González</t>
-  </si>
-  <si>
-    <t>Martínez</t>
-  </si>
-  <si>
-    <t>11411411D</t>
-  </si>
-  <si>
-    <t>Pedro</t>
-  </si>
-  <si>
-    <t>Ruiz</t>
-  </si>
-  <si>
-    <t>Fernández</t>
-  </si>
-  <si>
-    <t>11511511E</t>
-  </si>
-  <si>
-    <t>Marta</t>
-  </si>
-  <si>
-    <t>Pérez</t>
-  </si>
-  <si>
-    <t>Sánchez</t>
-  </si>
-  <si>
-    <t>11611611F</t>
-  </si>
-  <si>
-    <t>Luis</t>
-  </si>
-  <si>
-    <t>Díaz</t>
-  </si>
-  <si>
-    <t>11711711G</t>
-  </si>
-  <si>
-    <t>Sara</t>
-  </si>
-  <si>
-    <t>Martín</t>
-  </si>
-  <si>
-    <t>Vázquez</t>
-  </si>
-  <si>
-    <t>11811811H</t>
-  </si>
-  <si>
-    <t>Javier</t>
-  </si>
-  <si>
-    <t>Hernández</t>
-  </si>
-  <si>
-    <t>Castro</t>
-  </si>
-  <si>
-    <t>11911911J</t>
-  </si>
-  <si>
-    <t>Elena</t>
-  </si>
-  <si>
-    <t>Lopez</t>
-  </si>
-  <si>
-    <t>Bravo</t>
-  </si>
-  <si>
-    <t>12012012A</t>
-  </si>
-  <si>
-    <t>Oscar</t>
-  </si>
-  <si>
-    <t>Caballero</t>
-  </si>
-  <si>
-    <t>12112112B</t>
-  </si>
-  <si>
-    <t>Rosa</t>
-  </si>
-  <si>
-    <t>Jiménez</t>
-  </si>
-  <si>
-    <t>Villar</t>
-  </si>
-  <si>
-    <t>12212212C</t>
-  </si>
-  <si>
-    <t>Calle falsa 124</t>
-  </si>
-  <si>
-    <t>Valencia</t>
-  </si>
-  <si>
-    <t>Calle falsa 125</t>
-  </si>
-  <si>
-    <t>Calle falsa 126</t>
-  </si>
-  <si>
-    <t>Calle falsa 127</t>
-  </si>
-  <si>
-    <t>Calle falsa 128</t>
-  </si>
-  <si>
-    <t>Calle falsa 129</t>
-  </si>
-  <si>
-    <t>Calle falsa 130</t>
-  </si>
-  <si>
-    <t>Calle falsa 131</t>
-  </si>
-  <si>
-    <t>Calle falsa 132</t>
-  </si>
-  <si>
-    <t>Calle falsa 133</t>
-  </si>
-  <si>
-    <t>Calle falsa 134</t>
-  </si>
-  <si>
-    <t>Torrent</t>
   </si>
   <si>
     <t>País de la Direccion</t>
@@ -1394,8 +1226,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17676F3E-BBA5-4FF3-AAD8-13C6DEB73BA9}">
   <dimension ref="A1:Z76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="V1" sqref="V1:Z1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2:R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1446,16 +1278,16 @@
         <v>187</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>246</v>
+        <v>190</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>247</v>
+        <v>191</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>245</v>
+        <v>189</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>32</v>
@@ -1495,65 +1327,33 @@
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
-        <v>189</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>190</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>191</v>
-      </c>
-      <c r="D2" s="12">
-        <v>35960</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>192</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>193</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>193</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>40</v>
-      </c>
+      <c r="A2" s="10"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
       <c r="I2" s="8" t="str">
         <f>IF(H2="", "", VLOOKUP(H2, $Y$2:$Z$76, 2, FALSE))</f>
-        <v>MEX</v>
-      </c>
-      <c r="J2" s="13">
-        <v>123465780</v>
-      </c>
-      <c r="K2" s="9" t="s">
-        <v>35</v>
-      </c>
+        <v/>
+      </c>
+      <c r="J2" s="13"/>
+      <c r="K2" s="9"/>
       <c r="L2" s="8" t="str">
         <f>IF(K2="", "", VLOOKUP(K2, $Y$2:$Z$76, 2, FALSE))</f>
-        <v>ESP</v>
-      </c>
-      <c r="M2" s="9" t="s">
-        <v>232</v>
-      </c>
-      <c r="N2" s="9" t="s">
-        <v>233</v>
-      </c>
-      <c r="O2" s="9">
-        <v>46112</v>
-      </c>
-      <c r="P2" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="Q2" s="9">
-        <v>46112</v>
-      </c>
-      <c r="R2" s="9" t="s">
-        <v>249</v>
-      </c>
+        <v/>
+      </c>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="9"/>
       <c r="S2" s="11" t="str">
         <f>IF(R2="","",VLOOKUP(R2,$V$2:$W$16,2,FALSE))</f>
-        <v>BA</v>
+        <v/>
       </c>
       <c r="V2" s="7" t="s">
         <v>19</v>
@@ -1569,71 +1369,39 @@
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
-        <v>194</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>195</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>196</v>
-      </c>
-      <c r="D3" s="12">
-        <v>35024</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>192</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>197</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>197</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>35</v>
-      </c>
+      <c r="A3" s="10"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
       <c r="I3" s="8" t="str">
         <f t="shared" ref="I3:I66" si="0">IF(H3="", "", VLOOKUP(H3, $Y$2:$Z$76, 2, FALSE))</f>
-        <v>ESP</v>
-      </c>
-      <c r="J3" s="13">
-        <v>123465780</v>
-      </c>
-      <c r="K3" s="9" t="s">
-        <v>35</v>
-      </c>
+        <v/>
+      </c>
+      <c r="J3" s="13"/>
+      <c r="K3" s="9"/>
       <c r="L3" s="8" t="str">
         <f t="shared" ref="L3:L66" si="1">IF(K3="", "", VLOOKUP(K3, $Y$2:$Z$76, 2, FALSE))</f>
-        <v>ESP</v>
-      </c>
-      <c r="M3" s="9" t="s">
-        <v>234</v>
-      </c>
-      <c r="N3" s="9" t="s">
-        <v>233</v>
-      </c>
-      <c r="O3" s="9">
-        <v>46112</v>
-      </c>
-      <c r="P3" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="Q3" s="9">
-        <v>46112</v>
-      </c>
-      <c r="R3" s="9" t="s">
-        <v>255</v>
-      </c>
+        <v/>
+      </c>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9"/>
       <c r="S3" s="11" t="str">
         <f t="shared" ref="S3:S66" si="2">IF(R3="","",VLOOKUP(R3,$V$2:$W$16,2,FALSE))</f>
-        <v>PM</v>
+        <v/>
       </c>
       <c r="V3" s="7" t="s">
-        <v>249</v>
+        <v>193</v>
       </c>
       <c r="W3" s="14" t="s">
-        <v>248</v>
+        <v>192</v>
       </c>
       <c r="Y3" s="7" t="s">
         <v>36</v>
@@ -1643,71 +1411,39 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
-        <v>198</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>199</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>200</v>
-      </c>
-      <c r="D4" s="12">
-        <v>35529</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>192</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>35</v>
-      </c>
+      <c r="A4" s="10"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
       <c r="I4" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>ESP</v>
-      </c>
-      <c r="J4" s="13">
-        <v>123465780</v>
-      </c>
-      <c r="K4" s="9" t="s">
-        <v>35</v>
-      </c>
+        <v/>
+      </c>
+      <c r="J4" s="13"/>
+      <c r="K4" s="9"/>
       <c r="L4" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>ESP</v>
-      </c>
-      <c r="M4" s="9" t="s">
-        <v>235</v>
-      </c>
-      <c r="N4" s="9" t="s">
-        <v>233</v>
-      </c>
-      <c r="O4" s="9">
-        <v>46112</v>
-      </c>
-      <c r="P4" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="Q4" s="9">
-        <v>46112</v>
-      </c>
-      <c r="R4" s="9" t="s">
-        <v>13</v>
-      </c>
+        <v/>
+      </c>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="9"/>
       <c r="S4" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>HJ</v>
+        <v/>
       </c>
       <c r="V4" s="7" t="s">
-        <v>251</v>
+        <v>195</v>
       </c>
       <c r="W4" s="14" t="s">
-        <v>250</v>
+        <v>194</v>
       </c>
       <c r="Y4" s="7" t="s">
         <v>38</v>
@@ -1717,71 +1453,39 @@
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
-        <v>202</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>204</v>
-      </c>
-      <c r="D5" s="12">
-        <v>36196</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>192</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>205</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>205</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>35</v>
-      </c>
+      <c r="A5" s="10"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
       <c r="I5" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>ESP</v>
-      </c>
-      <c r="J5" s="13">
-        <v>123465780</v>
-      </c>
-      <c r="K5" s="9" t="s">
-        <v>35</v>
-      </c>
+        <v/>
+      </c>
+      <c r="J5" s="13"/>
+      <c r="K5" s="9"/>
       <c r="L5" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>ESP</v>
-      </c>
-      <c r="M5" s="9" t="s">
-        <v>236</v>
-      </c>
-      <c r="N5" s="9" t="s">
-        <v>233</v>
-      </c>
-      <c r="O5" s="9">
-        <v>46112</v>
-      </c>
-      <c r="P5" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="Q5" s="9">
-        <v>46112</v>
-      </c>
-      <c r="R5" s="9" t="s">
-        <v>21</v>
-      </c>
+        <v/>
+      </c>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="9"/>
+      <c r="R5" s="9"/>
       <c r="S5" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>NI</v>
+        <v/>
       </c>
       <c r="V5" s="7" t="s">
-        <v>253</v>
+        <v>197</v>
       </c>
       <c r="W5" s="14" t="s">
-        <v>252</v>
+        <v>196</v>
       </c>
       <c r="Y5" s="7" t="s">
         <v>40</v>
@@ -1791,59 +1495,29 @@
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
-        <v>206</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>208</v>
-      </c>
-      <c r="D6" s="12">
-        <v>35626</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>192</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>209</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>209</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>35</v>
-      </c>
+      <c r="A6" s="10"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
       <c r="I6" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>ESP</v>
-      </c>
-      <c r="J6" s="13">
-        <v>123465780</v>
-      </c>
-      <c r="K6" s="9" t="s">
-        <v>35</v>
-      </c>
+        <v/>
+      </c>
+      <c r="J6" s="13"/>
+      <c r="K6" s="9"/>
       <c r="L6" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>ESP</v>
-      </c>
-      <c r="M6" s="9" t="s">
-        <v>237</v>
-      </c>
-      <c r="N6" s="9" t="s">
-        <v>233</v>
-      </c>
-      <c r="O6" s="9">
-        <v>46112</v>
-      </c>
-      <c r="P6" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="Q6" s="9">
-        <v>46112</v>
-      </c>
+        <v/>
+      </c>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
       <c r="R6" s="9"/>
       <c r="S6" s="11" t="str">
         <f t="shared" si="2"/>
@@ -1863,65 +1537,33 @@
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
-        <v>210</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>191</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>211</v>
-      </c>
-      <c r="D7" s="12">
-        <v>35146</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>192</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>212</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>212</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>35</v>
-      </c>
+      <c r="A7" s="10"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
       <c r="I7" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>ESP</v>
-      </c>
-      <c r="J7" s="13">
-        <v>123465780</v>
-      </c>
-      <c r="K7" s="9" t="s">
-        <v>35</v>
-      </c>
+        <v/>
+      </c>
+      <c r="J7" s="13"/>
+      <c r="K7" s="9"/>
       <c r="L7" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>ESP</v>
-      </c>
-      <c r="M7" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="N7" s="9" t="s">
-        <v>233</v>
-      </c>
-      <c r="O7" s="9">
-        <v>46112</v>
-      </c>
-      <c r="P7" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="Q7" s="9">
-        <v>46112</v>
-      </c>
-      <c r="R7" s="9" t="s">
-        <v>23</v>
-      </c>
+        <v/>
+      </c>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="9"/>
       <c r="S7" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>SB</v>
+        <v/>
       </c>
       <c r="V7" s="7" t="s">
         <v>13</v>
@@ -1937,59 +1579,29 @@
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
-        <v>213</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>214</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>215</v>
-      </c>
-      <c r="D8" s="12">
-        <v>35063</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>192</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>216</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>216</v>
-      </c>
-      <c r="H8" s="9" t="s">
-        <v>35</v>
-      </c>
+      <c r="A8" s="10"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
       <c r="I8" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>ESP</v>
-      </c>
-      <c r="J8" s="13">
-        <v>123465780</v>
-      </c>
-      <c r="K8" s="9" t="s">
-        <v>35</v>
-      </c>
+        <v/>
+      </c>
+      <c r="J8" s="13"/>
+      <c r="K8" s="9"/>
       <c r="L8" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>ESP</v>
-      </c>
-      <c r="M8" s="9" t="s">
-        <v>239</v>
-      </c>
-      <c r="N8" s="9" t="s">
-        <v>233</v>
-      </c>
-      <c r="O8" s="9">
-        <v>46112</v>
-      </c>
-      <c r="P8" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="Q8" s="9">
-        <v>46112</v>
-      </c>
+        <v/>
+      </c>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
       <c r="R8" s="9"/>
       <c r="S8" s="11" t="str">
         <f t="shared" si="2"/>
@@ -2009,59 +1621,29 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
-        <v>217</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>219</v>
-      </c>
-      <c r="D9" s="12">
-        <v>36048</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>192</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="H9" s="9" t="s">
-        <v>35</v>
-      </c>
+      <c r="A9" s="10"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
       <c r="I9" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>ESP</v>
-      </c>
-      <c r="J9" s="13">
-        <v>123465780</v>
-      </c>
-      <c r="K9" s="9" t="s">
-        <v>35</v>
-      </c>
+        <v/>
+      </c>
+      <c r="J9" s="13"/>
+      <c r="K9" s="9"/>
       <c r="L9" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>ESP</v>
-      </c>
-      <c r="M9" s="9" t="s">
-        <v>240</v>
-      </c>
-      <c r="N9" s="9" t="s">
-        <v>233</v>
-      </c>
-      <c r="O9" s="9">
-        <v>46112</v>
-      </c>
-      <c r="P9" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="Q9" s="9">
-        <v>46112</v>
-      </c>
+        <v/>
+      </c>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9"/>
       <c r="R9" s="9"/>
       <c r="S9" s="11" t="str">
         <f t="shared" si="2"/>
@@ -2081,71 +1663,39 @@
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
-        <v>221</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>222</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="D10" s="12">
-        <v>35082</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>192</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="H10" s="9" t="s">
-        <v>35</v>
-      </c>
+      <c r="A10" s="10"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
       <c r="I10" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>ESP</v>
-      </c>
-      <c r="J10" s="13">
-        <v>123465780</v>
-      </c>
-      <c r="K10" s="9" t="s">
-        <v>35</v>
-      </c>
+        <v/>
+      </c>
+      <c r="J10" s="13"/>
+      <c r="K10" s="9"/>
       <c r="L10" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>ESP</v>
-      </c>
-      <c r="M10" s="9" t="s">
-        <v>241</v>
-      </c>
-      <c r="N10" s="9" t="s">
-        <v>233</v>
-      </c>
-      <c r="O10" s="9">
-        <v>46112</v>
-      </c>
-      <c r="P10" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="Q10" s="9">
-        <v>46112</v>
-      </c>
-      <c r="R10" s="9" t="s">
-        <v>257</v>
-      </c>
+        <v/>
+      </c>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="9"/>
+      <c r="R10" s="9"/>
       <c r="S10" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>SG</v>
+        <v/>
       </c>
       <c r="V10" s="7" t="s">
-        <v>255</v>
+        <v>199</v>
       </c>
       <c r="W10" s="14" t="s">
-        <v>254</v>
+        <v>198</v>
       </c>
       <c r="Y10" s="7" t="s">
         <v>50</v>
@@ -2155,59 +1705,29 @@
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
-        <v>225</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>219</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>226</v>
-      </c>
-      <c r="D11" s="12">
-        <v>35728</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>192</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>227</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>227</v>
-      </c>
-      <c r="H11" s="9" t="s">
-        <v>35</v>
-      </c>
+      <c r="A11" s="10"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
       <c r="I11" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>ESP</v>
-      </c>
-      <c r="J11" s="13">
-        <v>123465780</v>
-      </c>
-      <c r="K11" s="9" t="s">
-        <v>35</v>
-      </c>
+        <v/>
+      </c>
+      <c r="J11" s="13"/>
+      <c r="K11" s="9"/>
       <c r="L11" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>ESP</v>
-      </c>
-      <c r="M11" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="N11" s="9" t="s">
-        <v>233</v>
-      </c>
-      <c r="O11" s="9">
-        <v>46112</v>
-      </c>
-      <c r="P11" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="Q11" s="9">
-        <v>46112</v>
-      </c>
+        <v/>
+      </c>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="9"/>
       <c r="R11" s="9"/>
       <c r="S11" s="11" t="str">
         <f t="shared" si="2"/>
@@ -2227,69 +1747,39 @@
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
-        <v>228</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>229</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="D12" s="12">
-        <v>36231</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>192</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>231</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>231</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>35</v>
-      </c>
+      <c r="A12" s="10"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
       <c r="I12" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>ESP</v>
-      </c>
-      <c r="J12" s="13">
-        <v>123465780</v>
-      </c>
-      <c r="K12" s="9" t="s">
-        <v>35</v>
-      </c>
+        <v/>
+      </c>
+      <c r="J12" s="13"/>
+      <c r="K12" s="9"/>
       <c r="L12" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>ESP</v>
-      </c>
-      <c r="M12" s="9" t="s">
-        <v>243</v>
-      </c>
-      <c r="N12" s="9" t="s">
-        <v>233</v>
-      </c>
-      <c r="O12" s="9">
-        <v>46112</v>
-      </c>
-      <c r="P12" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="Q12" s="9">
-        <v>46112</v>
-      </c>
+        <v/>
+      </c>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="9"/>
       <c r="R12" s="9"/>
       <c r="S12" s="11" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="V12" s="7" t="s">
-        <v>257</v>
+        <v>201</v>
       </c>
       <c r="W12" s="14" t="s">
-        <v>256</v>
+        <v>200</v>
       </c>
       <c r="Y12" s="7" t="s">
         <v>54</v>
@@ -2370,7 +1860,7 @@
         <v/>
       </c>
       <c r="V14" s="7" t="s">
-        <v>258</v>
+        <v>202</v>
       </c>
       <c r="W14" s="14" t="s">
         <v>27</v>
@@ -4515,7 +4005,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="ZY1v2iNw6EN8erJKl5JD74FZACoWRhR8Ympr13Nw7cALScIf7Sm/Yr79JGAGPrM5NyXYgKlV65WCTaIoIug92Q==" saltValue="RCP0O+0lwcpYaN5D1CiQLg==" spinCount="100000" sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="5">
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D72" xr:uid="{5BEAB45D-33D4-49C6-8606-5A33F0D469D5}">

</xml_diff>